<commit_message>
Support companies per counters
</commit_message>
<xml_diff>
--- a/dist/prowess-frontend/assets/files/importing-sample.xlsx
+++ b/dist/prowess-frontend/assets/files/importing-sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -46,22 +46,34 @@
     <t>planPrice</t>
   </si>
   <si>
-    <t>importted succ</t>
-  </si>
-  <si>
-    <t>imported_succ@gmail.com</t>
-  </si>
-  <si>
-    <t>alika</t>
-  </si>
-  <si>
-    <t>Sfeir</t>
-  </si>
-  <si>
-    <t>Chinese</t>
+    <t>lastCounterValue</t>
+  </si>
+  <si>
+    <t>isPerCounter</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>optional_email@email.com</t>
+  </si>
+  <si>
+    <t>employeeUsername</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Floor</t>
   </si>
   <si>
     <t>4MB</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE</t>
   </si>
 </sst>
 </file>
@@ -69,13 +81,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -86,7 +110,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -118,28 +142,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,86 +485,100 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="15.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="9">
+        <v>96171234567</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4">
-        <v>3488924254</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="5">
-        <v>10</v>
+      <c r="K2" s="3">
+        <v>2419</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update importing sample Excel file
</commit_message>
<xml_diff>
--- a/dist/prowess-frontend/assets/files/importing-sample.xlsx
+++ b/dist/prowess-frontend/assets/files/importing-sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>planPrice</t>
+  </si>
+  <si>
+    <t>pricePerCounter</t>
   </si>
   <si>
     <t>lastCounterValue</t>
@@ -81,7 +84,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,18 +100,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -142,33 +139,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -485,24 +491,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="15.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="15" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="16" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="15" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -527,58 +534,64 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9">
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3">
         <v>96171234567</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="10">
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="11" t="s">
         <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="J2" s="3">
         <v>10</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="L2" s="10">
         <v>2419</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>19</v>
+      <c r="M2" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>